<commit_message>
Update to simulation parameters key
</commit_message>
<xml_diff>
--- a/Data/MSM4PCoD_SimulationParameters_V3.xlsx
+++ b/Data/MSM4PCoD_SimulationParameters_V3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ej45\Desktop\MSM4PCoD\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ej45/Documents/MSM4PCoD/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C51754C-B723-4649-8A69-3991747E3C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1065" windowWidth="4515" windowHeight="2025"/>
+    <workbookView xWindow="0" yWindow="1060" windowWidth="29400" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="108">
   <si>
     <t>nyears</t>
   </si>
@@ -334,9 +335,6 @@
   </si>
   <si>
     <t>NULL_20yrReal_wCalfData_2023-10-20</t>
-  </si>
-  <si>
-    <t>NULL_Actual_wCalfData_2023-10-20</t>
   </si>
   <si>
     <t>NULL_Ideal_2023-10-20</t>
@@ -357,7 +355,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -702,36 +700,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="T30" sqref="T30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="30.875" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="30.83203125" customWidth="1"/>
     <col min="8" max="8" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="31" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="29.875" customWidth="1"/>
+    <col min="13" max="13" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="29.83203125" customWidth="1"/>
     <col min="17" max="17" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>67</v>
       </c>
@@ -796,7 +794,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -864,7 +862,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -932,7 +930,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1000,7 +998,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -1068,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1136,7 +1134,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1204,7 +1202,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1272,7 +1270,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1340,7 +1338,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1408,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1476,7 +1474,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -1544,7 +1542,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1612,7 +1610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1680,7 +1678,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1748,7 +1746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1816,7 +1814,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1884,7 +1882,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -1952,7 +1950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -2020,7 +2018,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2088,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>15</v>
       </c>
@@ -2156,7 +2154,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -2224,7 +2222,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2292,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -2360,7 +2358,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2428,7 +2426,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2496,7 +2494,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2564,7 +2562,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2632,12 +2630,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q29" t="s">
         <v>99</v>
@@ -2646,7 +2644,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>68</v>
       </c>
@@ -2663,10 +2661,10 @@
         <v>101</v>
       </c>
       <c r="F30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H30" t="s">
         <v>86</v>
@@ -2690,10 +2688,10 @@
         <v>102</v>
       </c>
       <c r="O30" t="s">
+        <v>106</v>
+      </c>
+      <c r="P30" t="s">
         <v>107</v>
-      </c>
-      <c r="P30" t="s">
-        <v>108</v>
       </c>
       <c r="Q30" t="s">
         <v>81</v>
@@ -2703,9 +2701,6 @@
       </c>
       <c r="S30" t="s">
         <v>84</v>
-      </c>
-      <c r="T30" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2714,16 +2709,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2731,7 +2726,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2739,7 +2734,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2747,7 +2742,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2755,7 +2750,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2763,7 +2758,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2771,7 +2766,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2779,7 +2774,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2787,7 +2782,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -2795,7 +2790,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2803,7 +2798,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -2811,7 +2806,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2819,7 +2814,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2827,7 +2822,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2835,7 +2830,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2843,7 +2838,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -2851,7 +2846,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2859,7 +2854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -2867,7 +2862,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2875,7 +2870,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2883,7 +2878,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2891,7 +2886,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2899,7 +2894,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2907,7 +2902,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2915,7 +2910,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2923,7 +2918,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2931,7 +2926,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2939,7 +2934,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -2947,7 +2942,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -2955,7 +2950,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>56</v>
       </c>
@@ -2963,7 +2958,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>57</v>
       </c>
@@ -2971,7 +2966,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Added IDs for "actual" scenario
</commit_message>
<xml_diff>
--- a/Data/MSM4PCoD_SimulationParameters_V3.xlsx
+++ b/Data/MSM4PCoD_SimulationParameters_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ej45/Documents/MSM4PCoD/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C51754C-B723-4649-8A69-3991747E3C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A633D3D-6339-6A4F-B014-5023378A7C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1060" windowWidth="29400" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-220" yWindow="740" windowWidth="29400" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="111">
   <si>
     <t>nyears</t>
   </si>
@@ -350,6 +350,15 @@
   </si>
   <si>
     <t>D50B_20yrReal_2023-10-23</t>
+  </si>
+  <si>
+    <t>NULL_Actual_wCalfData_2023-10-24</t>
+  </si>
+  <si>
+    <t>D50AB_Actual_wCalfData_2023-10-24</t>
+  </si>
+  <si>
+    <t>D50B_Actual_2023-10-24</t>
   </si>
 </sst>
 </file>
@@ -704,9 +713,9 @@
   <dimension ref="A1:V30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="T30" sqref="T30"/>
+      <selection pane="bottomLeft" activeCell="V31" sqref="V31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,6 +736,8 @@
     <col min="18" max="18" width="31.83203125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="30.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.2">
@@ -2701,6 +2712,15 @@
       </c>
       <c r="S30" t="s">
         <v>84</v>
+      </c>
+      <c r="T30" t="s">
+        <v>108</v>
+      </c>
+      <c r="U30" t="s">
+        <v>109</v>
+      </c>
+      <c r="V30" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed mistake with "actual" sim pars
</commit_message>
<xml_diff>
--- a/Data/MSM4PCoD_SimulationParameters_V3.xlsx
+++ b/Data/MSM4PCoD_SimulationParameters_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ej45/Documents/MSM4PCoD/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A633D3D-6339-6A4F-B014-5023378A7C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B25961-8D60-0049-A72B-921F7AE97D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-220" yWindow="740" windowWidth="29400" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="108">
   <si>
     <t>nyears</t>
   </si>
@@ -350,15 +350,6 @@
   </si>
   <si>
     <t>D50B_20yrReal_2023-10-23</t>
-  </si>
-  <si>
-    <t>NULL_Actual_wCalfData_2023-10-24</t>
-  </si>
-  <si>
-    <t>D50AB_Actual_wCalfData_2023-10-24</t>
-  </si>
-  <si>
-    <t>D50B_Actual_2023-10-24</t>
   </si>
 </sst>
 </file>
@@ -712,10 +703,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="V31" sqref="V31"/>
+      <selection pane="bottomLeft" activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2156,13 +2147,13 @@
         <v>35</v>
       </c>
       <c r="T21">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="U21">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="V21">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
@@ -2224,13 +2215,13 @@
         <v>65</v>
       </c>
       <c r="T22">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="U22">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="V22">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
@@ -2712,15 +2703,6 @@
       </c>
       <c r="S30" t="s">
         <v>84</v>
-      </c>
-      <c r="T30" t="s">
-        <v>108</v>
-      </c>
-      <c r="U30" t="s">
-        <v>109</v>
-      </c>
-      <c r="V30" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>